<commit_message>
Document management in voucher repository (Build 432)
</commit_message>
<xml_diff>
--- a/doc/Analysis/TahlilTadbirWeb.xlsx
+++ b/doc/Analysis/TahlilTadbirWeb.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ورود به برنامه " sheetId="4" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="سند حسابداری " sheetId="5" r:id="rId5"/>
     <sheet name="گزارشات حسابداری  " sheetId="6" r:id="rId6"/>
     <sheet name="کارتابل " sheetId="7" r:id="rId7"/>
+    <sheet name="داشبورد" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="313">
   <si>
     <t xml:space="preserve">موضوع </t>
   </si>
@@ -757,13 +758,6 @@
   </si>
   <si>
     <t xml:space="preserve">دفاتر قانونی </t>
-  </si>
-  <si>
-    <t>دفتر روزنامه
-دفتر کل
- خلاصه اسناد
- خلاصه سند روزانه
- خلاصه سند ماهانه</t>
   </si>
   <si>
     <t xml:space="preserve">صورت های مالی </t>
@@ -1163,6 +1157,223 @@
   <si>
     <t xml:space="preserve">تعیین سن بدهی ها </t>
   </si>
+  <si>
+    <t xml:space="preserve">نسبت جاری </t>
+  </si>
+  <si>
+    <t xml:space="preserve">دارایی های جاری ÷ بدهی های جاری </t>
+  </si>
+  <si>
+    <t xml:space="preserve">نسبت آنی </t>
+  </si>
+  <si>
+    <t xml:space="preserve">دارایی‌های آنی / بدهی‌های جاری 
+دارایی آنی = بانک + صندوق+ اسناد دریافتنی + حساب های دریافتنی </t>
+  </si>
+  <si>
+    <t xml:space="preserve">نسبت نقدی  </t>
+  </si>
+  <si>
+    <t>(وجه نقد + اوراق بهادار قابل تبدیل)   /  بدهی‌های جاری</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تصویر فرم </t>
+  </si>
+  <si>
+    <t xml:space="preserve">فروش </t>
+  </si>
+  <si>
+    <t xml:space="preserve">گردش بستانکارحساب فروش  به صورت نموداری روزانه _ هفتگی _ ماهانه 
+یا 
+مانده حساب صندوق </t>
+  </si>
+  <si>
+    <t xml:space="preserve">نمایش ساعت عقربه ای </t>
+  </si>
+  <si>
+    <t xml:space="preserve">نمایش ساعت </t>
+  </si>
+  <si>
+    <t xml:space="preserve">نمایش متن </t>
+  </si>
+  <si>
+    <t>نکته روز :
+یا 
+کارهای دریافتی جدید از کارتابل 
+کارهای دریافتی با اقدام جدید 
+کارهای ارسالی با اقدام جدید</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مدیریت اسناد </t>
+  </si>
+  <si>
+    <t>دفتر روزنامه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">دفتر کل _ دفتر حساب </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ خلاصه سند روزانه
+ خلاصه سند ماهانه</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> خلاصه اسناد</t>
+  </si>
+  <si>
+    <t>دفاتر قانونی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تراز آزمایشی </t>
+  </si>
+  <si>
+    <t xml:space="preserve">درحال انجام </t>
+  </si>
+  <si>
+    <r>
+      <t>ستون ها شامل :
+شماره سند _ تاریخ _ کاربر ایجاد کننده _ وضعیت ثبت(یادداشت، ثبت، ثبت قطعی) _ وضعیت تراز (تراز، ناتراز)_ ماخذ سند(سند افتتاحیه ، سند اختتامیه، سند عادی) _ شرح سند _</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve"> رفرنس _ تایید کننده _ تصویب کننده</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+مطابق ردیف های سند :
+ردیف _ تاریخ _ شماره سند _ شماره حساب </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>( فقط کد حساب های اصلی بدون سطوح شناور)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve"> _ عنوان حساب _ شرح _ بدهکار</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>(مبلغ)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve"> _ بستانکار </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>(مبلغ)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ساده _ مطابق ردیفهای سند:
+ردیف_ شماره سند  _ تاریخ  _ شرح </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">(شرح سطر سند) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>_ بدهکار</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">(مبلغ) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">_ بستانکار </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>(مبلغ)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">_ مانده </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>(بدهکار - بستانکار(اگر بستانکار بود عدد منفی نمایش داده شود))</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1171,7 +1382,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-2000401]0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1242,8 +1453,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="B Nazanin"/>
+      <charset val="178"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="B Nazanin"/>
+      <charset val="178"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1280,8 +1504,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1375,12 +1617,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
@@ -1542,6 +1799,21 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1553,13 +1825,81 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="41">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="B Nazanin"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="B Nazanin"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="B Nazanin"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="B Nazanin"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="B Nazanin"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2046,79 +2386,370 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4747532</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1476088</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9985053418" y="314325"/>
+          <a:ext cx="4490357" cy="1399888"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>35719</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>35718</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4869656</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1587803</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9945933562" y="1952624"/>
+          <a:ext cx="4833937" cy="1552085"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>130970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4631532</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2063340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9946171686" y="3738564"/>
+          <a:ext cx="4393407" cy="1932370"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1850571</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>120760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4068536</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>524212</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="61098" t="14114" r="11445" b="46902"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10056575130" y="385343"/>
+          <a:ext cx="2217965" cy="2244952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>5442858</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3374572</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect l="959" t="14100" r="47051" b="41907"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10029824999" y="2204357"/>
+          <a:ext cx="5157107" cy="3184072"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1847850</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4019550</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2457450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:srcRect l="2664" t="58628" r="75363" b="7681"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9986676750" y="6477000"/>
+          <a:ext cx="2171700" cy="2419350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>875891</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>214312</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4619625</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2608844</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10142696250" y="9215437"/>
+          <a:ext cx="3743734" cy="2394532"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D30" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D30" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="A1:D30"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="وضعیت" dataDxfId="33"/>
-    <tableColumn id="2" name="موضوع " dataDxfId="32"/>
-    <tableColumn id="3" name="توضیحات " dataDxfId="31"/>
-    <tableColumn id="4" name="توضیحات 2" dataDxfId="30"/>
+    <tableColumn id="1" name="وضعیت" dataDxfId="38"/>
+    <tableColumn id="2" name="موضوع " dataDxfId="37"/>
+    <tableColumn id="3" name="توضیحات " dataDxfId="36"/>
+    <tableColumn id="4" name="توضیحات 2" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="A1:D24"/>
   <tableColumns count="4">
-    <tableColumn id="2" name="وضعیت" dataDxfId="27"/>
-    <tableColumn id="3" name="موضوع " dataDxfId="26"/>
-    <tableColumn id="4" name="توضیحات " dataDxfId="25"/>
-    <tableColumn id="5" name="توضیحات 2" dataDxfId="24"/>
+    <tableColumn id="2" name="وضعیت" dataDxfId="32"/>
+    <tableColumn id="3" name="موضوع " dataDxfId="31"/>
+    <tableColumn id="4" name="توضیحات " dataDxfId="30"/>
+    <tableColumn id="5" name="توضیحات 2" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:D23" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:D23" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A2:D23"/>
   <tableColumns count="4">
-    <tableColumn id="2" name="وضعیت" dataDxfId="21"/>
-    <tableColumn id="3" name="موضوع " dataDxfId="20"/>
-    <tableColumn id="4" name="توضیحات " dataDxfId="19"/>
-    <tableColumn id="5" name="توضیحات 2" dataDxfId="18"/>
+    <tableColumn id="2" name="وضعیت" dataDxfId="26"/>
+    <tableColumn id="3" name="موضوع " dataDxfId="25"/>
+    <tableColumn id="4" name="توضیحات " dataDxfId="24"/>
+    <tableColumn id="5" name="توضیحات 2" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D38" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D38" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:D38"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="وضعیت" dataDxfId="15"/>
-    <tableColumn id="2" name="موضوع " dataDxfId="14"/>
-    <tableColumn id="3" name="توضیحات " dataDxfId="13"/>
-    <tableColumn id="4" name="توضیحات 2" dataDxfId="12"/>
+    <tableColumn id="1" name="وضعیت" dataDxfId="20"/>
+    <tableColumn id="2" name="موضوع " dataDxfId="19"/>
+    <tableColumn id="3" name="توضیحات " dataDxfId="18"/>
+    <tableColumn id="4" name="توضیحات 2" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A1:D37" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:D37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A1:D41" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:D41"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="وضعیت" dataDxfId="9"/>
-    <tableColumn id="2" name="موضوع " dataDxfId="8"/>
-    <tableColumn id="3" name="توضیحات " dataDxfId="7"/>
-    <tableColumn id="4" name="توضیحات 2" dataDxfId="6"/>
+    <tableColumn id="1" name="وضعیت" dataDxfId="14"/>
+    <tableColumn id="2" name="موضوع " dataDxfId="13"/>
+    <tableColumn id="3" name="توضیحات " dataDxfId="12"/>
+    <tableColumn id="4" name="توضیحات 2" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table267" displayName="Table267" ref="A1:D39" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table267" displayName="Table267" ref="A1:D39" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:D39"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="وضعیت" dataDxfId="3"/>
-    <tableColumn id="2" name="موضوع " dataDxfId="2"/>
-    <tableColumn id="3" name="توضیحات " dataDxfId="1"/>
-    <tableColumn id="4" name="توضیحات 2" dataDxfId="0"/>
+    <tableColumn id="1" name="وضعیت" dataDxfId="8"/>
+    <tableColumn id="2" name="موضوع " dataDxfId="7"/>
+    <tableColumn id="3" name="توضیحات " dataDxfId="6"/>
+    <tableColumn id="4" name="توضیحات 2" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table2678" displayName="Table2678" ref="A1:C39" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C39"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="وضعیت" dataDxfId="2"/>
+    <tableColumn id="2" name="موضوع " dataDxfId="1"/>
+    <tableColumn id="3" name="توضیحات " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2476,7 +3107,7 @@
   <dimension ref="A1:H140"/>
   <sheetViews>
     <sheetView rightToLeft="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2525,7 +3156,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D3" s="46" t="s">
         <v>174</v>
@@ -2597,14 +3228,14 @@
         <v>10</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D10" s="19"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="19"/>
       <c r="B11" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>20</v>
@@ -2615,7 +3246,7 @@
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D12" s="19"/>
     </row>
@@ -2667,7 +3298,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D17" s="19"/>
     </row>
@@ -2677,7 +3308,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D18" s="19"/>
     </row>
@@ -2687,7 +3318,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D19" s="19"/>
     </row>
@@ -2697,11 +3328,11 @@
         <v>15</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D20" s="19"/>
     </row>
-    <row r="21" spans="1:4" ht="75">
+    <row r="21" spans="1:4" ht="89.25" customHeight="1">
       <c r="A21" s="19"/>
       <c r="B21" s="16" t="s">
         <v>16</v>
@@ -2711,7 +3342,7 @@
       </c>
       <c r="D21" s="19"/>
     </row>
-    <row r="22" spans="1:4" ht="115.5" customHeight="1">
+    <row r="22" spans="1:4" ht="141.75" customHeight="1">
       <c r="A22" s="19"/>
       <c r="B22" s="16" t="s">
         <v>177</v>
@@ -2760,8 +3391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C124"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2771,11 +3402,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" thickBot="1">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="64"/>
     </row>
     <row r="2" spans="1:3" ht="19.5" thickBot="1">
       <c r="A2" s="22" t="s">
@@ -3936,13 +4567,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="65" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
@@ -4083,7 +4714,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -4120,7 +4751,7 @@
         <v>210</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="37.5">
@@ -4144,7 +4775,7 @@
         <v>212</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="37.5">
@@ -4208,7 +4839,7 @@
         <v>213</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>219</v>
@@ -4227,7 +4858,7 @@
         <v>215</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="37.5">
@@ -4278,10 +4909,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -4289,7 +4920,309 @@
     <col min="1" max="1" width="11" style="14" customWidth="1"/>
     <col min="2" max="2" width="22.140625" style="14" customWidth="1"/>
     <col min="3" max="3" width="69" style="13" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="77.42578125" style="14" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" ht="132" customHeight="1">
+      <c r="A2" s="54" t="s">
+        <v>309</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D2" s="58" t="s">
+        <v>310</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" ht="132.75" customHeight="1">
+      <c r="A3" s="54"/>
+      <c r="B3" s="54" t="s">
+        <v>307</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>311</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" ht="180" customHeight="1">
+      <c r="A4" s="54"/>
+      <c r="B4" s="54" t="s">
+        <v>307</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>312</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="54"/>
+      <c r="B5" s="54" t="s">
+        <v>307</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="D5" s="58"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:7" ht="93.75">
+      <c r="B6" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" ht="112.5">
+      <c r="B7" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="75">
+      <c r="B8" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="75">
+      <c r="B13" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="37.5">
+      <c r="C21" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="C22" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" s="8"/>
+    </row>
+    <row r="37" spans="3:3">
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" s="8"/>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" s="8"/>
+    </row>
+    <row r="40" spans="3:3">
+      <c r="C40" s="8"/>
+    </row>
+    <row r="41" spans="3:3">
+      <c r="C41" s="8"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
+      <formula1>",درحال انجام ,نیاز به بررسی,موکول به آینده,رد شده ,تایید شده,"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G39"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <cols>
+    <col min="1" max="1" width="11" style="14" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="14" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" style="13" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
@@ -4310,197 +5243,183 @@
       <c r="F1" s="10"/>
       <c r="G1" s="12"/>
     </row>
-    <row r="2" spans="1:7" ht="93.75">
-      <c r="B2" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="D2" s="15"/>
-    </row>
-    <row r="3" spans="1:7" ht="112.5">
-      <c r="B3" s="10"/>
-      <c r="C3" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="75">
-      <c r="B4" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+    <row r="2" spans="1:7" ht="75">
+      <c r="B2" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="37.5">
+      <c r="B3" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="50"/>
+      <c r="B4" s="50" t="s">
+        <v>267</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>278</v>
+      </c>
+      <c r="D4" s="51"/>
+    </row>
+    <row r="5" spans="1:7" ht="112.5">
       <c r="B5" s="10" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="105">
       <c r="B6" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>268</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="112.5">
       <c r="B7" s="10" t="s">
-        <v>229</v>
+        <v>280</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>239</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="B8" s="10" t="s">
-        <v>227</v>
+        <v>270</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="75">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="99">
       <c r="B9" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="B11" s="14" t="s">
-        <v>231</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="B12" s="14" t="s">
-        <v>232</v>
+        <v>273</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="115.5">
+      <c r="A10" s="53"/>
+      <c r="B10" s="54" t="s">
+        <v>274</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>275</v>
+      </c>
+      <c r="D10" s="49"/>
+    </row>
+    <row r="11" spans="1:7" ht="206.25">
+      <c r="B11" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>283</v>
+      </c>
+      <c r="D11" s="51"/>
+    </row>
+    <row r="12" spans="1:7" ht="75">
+      <c r="B12" s="10" t="s">
+        <v>262</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>244</v>
+        <v>263</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="B13" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>288</v>
-      </c>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="B14" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>289</v>
-      </c>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="B15" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>247</v>
-      </c>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="B16" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" ht="37.5">
-      <c r="C17" s="4" t="s">
-        <v>249</v>
-      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="3:3">
-      <c r="C18" s="4" t="s">
-        <v>250</v>
-      </c>
+      <c r="C18" s="4"/>
     </row>
     <row r="19" spans="3:3">
-      <c r="C19" s="11"/>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="3:3">
-      <c r="C20" s="8"/>
+      <c r="C20" s="4"/>
     </row>
     <row r="21" spans="3:3">
-      <c r="C21" s="8"/>
+      <c r="C21" s="11"/>
     </row>
     <row r="22" spans="3:3">
-      <c r="C22" s="8"/>
+      <c r="C22" s="49"/>
     </row>
     <row r="23" spans="3:3">
-      <c r="C23" s="8"/>
+      <c r="C23" s="49"/>
     </row>
     <row r="24" spans="3:3">
-      <c r="C24" s="8"/>
+      <c r="C24" s="49"/>
     </row>
     <row r="25" spans="3:3">
-      <c r="C25" s="8"/>
+      <c r="C25" s="49"/>
     </row>
     <row r="26" spans="3:3">
-      <c r="C26" s="8"/>
+      <c r="C26" s="49"/>
     </row>
     <row r="27" spans="3:3">
-      <c r="C27" s="8"/>
+      <c r="C27" s="49"/>
     </row>
     <row r="28" spans="3:3">
-      <c r="C28" s="8"/>
+      <c r="C28" s="49"/>
     </row>
     <row r="29" spans="3:3">
-      <c r="C29" s="8"/>
+      <c r="C29" s="49"/>
     </row>
     <row r="30" spans="3:3">
-      <c r="C30" s="8"/>
+      <c r="C30" s="49"/>
     </row>
     <row r="31" spans="3:3">
-      <c r="C31" s="8"/>
+      <c r="C31" s="49"/>
     </row>
     <row r="32" spans="3:3">
-      <c r="C32" s="8"/>
+      <c r="C32" s="49"/>
     </row>
     <row r="33" spans="3:3">
-      <c r="C33" s="8"/>
+      <c r="C33" s="49"/>
     </row>
     <row r="34" spans="3:3">
-      <c r="C34" s="8"/>
+      <c r="C34" s="49"/>
     </row>
     <row r="35" spans="3:3">
-      <c r="C35" s="8"/>
+      <c r="C35" s="49"/>
     </row>
     <row r="36" spans="3:3">
-      <c r="C36" s="8"/>
+      <c r="C36" s="49"/>
     </row>
     <row r="37" spans="3:3">
-      <c r="C37" s="8"/>
+      <c r="C37" s="49"/>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" s="49"/>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" s="49"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -4516,12 +5435,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView rightToLeft="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -4529,11 +5448,11 @@
     <col min="1" max="1" width="11" style="14" customWidth="1"/>
     <col min="2" max="2" width="33.7109375" style="14" customWidth="1"/>
     <col min="3" max="3" width="75.7109375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="56.42578125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="90.7109375" style="59" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21">
+    <row r="1" spans="1:6" ht="21">
       <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
@@ -4543,119 +5462,96 @@
       <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>25</v>
+      <c r="D1" s="60" t="s">
+        <v>295</v>
       </c>
       <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="12"/>
-    </row>
-    <row r="2" spans="1:7" ht="75">
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" ht="80.25" customHeight="1">
       <c r="B2" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="C2" s="49" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="37.5">
+        <v>289</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>290</v>
+      </c>
+      <c r="D2" s="66"/>
+    </row>
+    <row r="3" spans="1:6" ht="65.25" customHeight="1">
       <c r="B3" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="C3" s="49" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>291</v>
+      </c>
+      <c r="C3" s="57" t="s">
+        <v>292</v>
+      </c>
+      <c r="D3" s="66"/>
+    </row>
+    <row r="4" spans="1:6" ht="45.75" customHeight="1">
       <c r="A4" s="50"/>
       <c r="B4" s="50" t="s">
-        <v>268</v>
-      </c>
-      <c r="C4" s="49" t="s">
-        <v>279</v>
-      </c>
-      <c r="D4" s="51"/>
-    </row>
-    <row r="5" spans="1:7" ht="112.5">
+        <v>293</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="D4" s="66"/>
+    </row>
+    <row r="5" spans="1:6" ht="292.5" customHeight="1">
       <c r="B5" s="10" t="s">
-        <v>267</v>
+        <v>296</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="105">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="204.75" customHeight="1">
       <c r="B6" s="10" t="s">
-        <v>269</v>
+        <v>298</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="112.5">
+        <v>299</v>
+      </c>
+      <c r="D6" s="61"/>
+    </row>
+    <row r="7" spans="1:6" ht="243" customHeight="1">
       <c r="B7" s="10" t="s">
-        <v>281</v>
+        <v>300</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="99">
-      <c r="B9" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="C9" s="56" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="115.5">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="10"/>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="10"/>
+      <c r="C9" s="56"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="53"/>
-      <c r="B10" s="54" t="s">
-        <v>275</v>
-      </c>
-      <c r="C10" s="55" t="s">
-        <v>276</v>
-      </c>
-      <c r="D10" s="49"/>
-    </row>
-    <row r="11" spans="1:7" ht="206.25">
-      <c r="B11" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="C11" s="48" t="s">
-        <v>284</v>
-      </c>
-      <c r="D11" s="51"/>
-    </row>
-    <row r="12" spans="1:7" ht="75">
-      <c r="B12" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="B10" s="54"/>
+      <c r="C10" s="55"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" s="10"/>
+      <c r="C11" s="48"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12" s="10"/>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:6">
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:6">
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:6">
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:6">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
     </row>
@@ -4675,60 +5571,63 @@
       <c r="C21" s="11"/>
     </row>
     <row r="22" spans="3:3">
-      <c r="C22" s="49"/>
+      <c r="C22" s="57"/>
     </row>
     <row r="23" spans="3:3">
-      <c r="C23" s="49"/>
+      <c r="C23" s="57"/>
     </row>
     <row r="24" spans="3:3">
-      <c r="C24" s="49"/>
+      <c r="C24" s="57"/>
     </row>
     <row r="25" spans="3:3">
-      <c r="C25" s="49"/>
+      <c r="C25" s="57"/>
     </row>
     <row r="26" spans="3:3">
-      <c r="C26" s="49"/>
+      <c r="C26" s="57"/>
     </row>
     <row r="27" spans="3:3">
-      <c r="C27" s="49"/>
+      <c r="C27" s="57"/>
     </row>
     <row r="28" spans="3:3">
-      <c r="C28" s="49"/>
+      <c r="C28" s="57"/>
     </row>
     <row r="29" spans="3:3">
-      <c r="C29" s="49"/>
+      <c r="C29" s="57"/>
     </row>
     <row r="30" spans="3:3">
-      <c r="C30" s="49"/>
+      <c r="C30" s="57"/>
     </row>
     <row r="31" spans="3:3">
-      <c r="C31" s="49"/>
+      <c r="C31" s="57"/>
     </row>
     <row r="32" spans="3:3">
-      <c r="C32" s="49"/>
+      <c r="C32" s="57"/>
     </row>
     <row r="33" spans="3:3">
-      <c r="C33" s="49"/>
+      <c r="C33" s="57"/>
     </row>
     <row r="34" spans="3:3">
-      <c r="C34" s="49"/>
+      <c r="C34" s="57"/>
     </row>
     <row r="35" spans="3:3">
-      <c r="C35" s="49"/>
+      <c r="C35" s="57"/>
     </row>
     <row r="36" spans="3:3">
-      <c r="C36" s="49"/>
+      <c r="C36" s="57"/>
     </row>
     <row r="37" spans="3:3">
-      <c r="C37" s="49"/>
+      <c r="C37" s="57"/>
     </row>
     <row r="38" spans="3:3">
-      <c r="C38" s="49"/>
+      <c r="C38" s="57"/>
     </row>
     <row r="39" spans="3:3">
-      <c r="C39" s="49"/>
+      <c r="C39" s="57"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:D4"/>
+  </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1">
       <formula1>",نیاز به بررسی,موکول به آینده,رد شده ,تایید شده,"</formula1>
@@ -4736,8 +5635,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dashboard API base implementation + doc update (Build 442)
</commit_message>
<xml_diff>
--- a/doc/Analysis/TahlilTadbirWeb.xlsx
+++ b/doc/Analysis/TahlilTadbirWeb.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ورود به برنامه " sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="323">
   <si>
     <t xml:space="preserve">موضوع </t>
   </si>
@@ -1161,9 +1161,6 @@
     <t xml:space="preserve">نسبت جاری </t>
   </si>
   <si>
-    <t xml:space="preserve">دارایی های جاری ÷ بدهی های جاری </t>
-  </si>
-  <si>
     <t xml:space="preserve">نسبت آنی </t>
   </si>
   <si>
@@ -1181,11 +1178,6 @@
   </si>
   <si>
     <t xml:space="preserve">فروش </t>
-  </si>
-  <si>
-    <t xml:space="preserve">گردش بستانکارحساب فروش  به صورت نموداری روزانه _ هفتگی _ ماهانه 
-یا 
-مانده حساب صندوق </t>
   </si>
   <si>
     <t xml:space="preserve">نمایش ساعت عقربه ای </t>
@@ -1374,6 +1366,88 @@
       <t>(بدهکار - بستانکار(اگر بستانکار بود عدد منفی نمایش داده شود))</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">دارایی های جاری </t>
+  </si>
+  <si>
+    <t xml:space="preserve">داراییهای غیر جاری </t>
+  </si>
+  <si>
+    <t xml:space="preserve">بدهی های جاری </t>
+  </si>
+  <si>
+    <t>بدهی های غیر جاری</t>
+  </si>
+  <si>
+    <t xml:space="preserve">حقوق صاحبان سرمایه </t>
+  </si>
+  <si>
+    <t xml:space="preserve">سایر درآمد ها </t>
+  </si>
+  <si>
+    <t xml:space="preserve">هزینه های عملیاتی </t>
+  </si>
+  <si>
+    <t xml:space="preserve">هزینه های غیر عملیاتی </t>
+  </si>
+  <si>
+    <t xml:space="preserve">رابط </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">گردش </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>ناخالص فروش</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>: گردش بستانکار  حساب فروش  
+گردش</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve"> خالص فروش:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve"> گردش بستانکار حساب فروش - گردش حساب بدهکار برگشت از فروش  -  بدهکار حساب  تخفیفات فروش 
+  به صورت نموداری روزانه _ هفتگی _ ماهانه 
+یا 
+مانده حساب صندوق </t>
+    </r>
+  </si>
+  <si>
+    <t>دارایی های جاری(گردش خالص )  ÷ بدهی های جاری (گردش خالص )</t>
+  </si>
+  <si>
+    <t>دارایی جاری ؟؟
+هزینه عملیاتی ؟؟
+قیمت تمام شده ؟؟</t>
+  </si>
 </sst>
 </file>
 
@@ -1382,7 +1456,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-2000401]0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1466,8 +1540,32 @@
       <name val="B Nazanin"/>
       <charset val="178"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1522,8 +1620,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8C4E4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1558,32 +1680,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1632,12 +1734,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
@@ -1701,71 +1851,50 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
@@ -1805,28 +1934,60 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2372,6 +2533,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE8C4E4"/>
       <color rgb="FF9966FF"/>
     </mruColors>
   </colors>
@@ -3158,7 +3320,7 @@
       <c r="C3" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="39" t="s">
         <v>174</v>
       </c>
     </row>
@@ -3170,7 +3332,7 @@
       <c r="C4" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="D4" s="47"/>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="1:4" ht="56.25">
       <c r="A5" s="19"/>
@@ -3389,1159 +3551,1324 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C124"/>
+  <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85:A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" thickBot="1">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A1" s="66" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="64"/>
-    </row>
-    <row r="2" spans="1:3" ht="19.5" thickBot="1">
-      <c r="A2" s="22" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="67"/>
+    </row>
+    <row r="2" spans="1:4" ht="19.5" thickBot="1">
+      <c r="A2" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="C2" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="D2" s="24" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75">
-      <c r="A3" s="25">
+    <row r="3" spans="1:4" ht="18.75">
+      <c r="A3" s="68" t="s">
+        <v>311</v>
+      </c>
+      <c r="B3" s="27">
         <v>111</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="C3" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="27"/>
-    </row>
-    <row r="4" spans="1:3" ht="18.75">
-      <c r="A4" s="25">
+      <c r="D3" s="26"/>
+    </row>
+    <row r="4" spans="1:4" ht="18.75">
+      <c r="A4" s="68"/>
+      <c r="B4" s="27">
         <v>111001</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="27"/>
-    </row>
-    <row r="5" spans="1:3" ht="18.75">
-      <c r="A5" s="25">
+      <c r="D4" s="26"/>
+    </row>
+    <row r="5" spans="1:4" ht="18.75">
+      <c r="A5" s="68"/>
+      <c r="B5" s="27">
         <v>1110010001</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="C5" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="27"/>
-    </row>
-    <row r="6" spans="1:3" ht="18.75">
-      <c r="A6" s="25">
+      <c r="D5" s="26"/>
+    </row>
+    <row r="6" spans="1:4" ht="18.75">
+      <c r="A6" s="68"/>
+      <c r="B6" s="27">
         <v>111002</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="C6" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="27"/>
-    </row>
-    <row r="7" spans="1:3" ht="18.75">
-      <c r="A7" s="29">
+      <c r="D6" s="26"/>
+    </row>
+    <row r="7" spans="1:4" ht="18.75">
+      <c r="A7" s="68"/>
+      <c r="B7" s="55">
         <v>111003</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="C7" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="27"/>
-    </row>
-    <row r="8" spans="1:3" ht="18.75">
-      <c r="A8" s="25">
+      <c r="D7" s="26"/>
+    </row>
+    <row r="8" spans="1:4" ht="18.75">
+      <c r="A8" s="68"/>
+      <c r="B8" s="27">
         <v>112</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="27"/>
-    </row>
-    <row r="9" spans="1:3" ht="18.75">
-      <c r="A9" s="25">
+      <c r="D8" s="26"/>
+    </row>
+    <row r="9" spans="1:4" ht="18.75">
+      <c r="A9" s="68"/>
+      <c r="B9" s="27">
         <v>112001</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="C9" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="27"/>
-    </row>
-    <row r="10" spans="1:3" ht="18.75">
-      <c r="A10" s="25">
+      <c r="D9" s="26"/>
+    </row>
+    <row r="10" spans="1:4" ht="18.75">
+      <c r="A10" s="68"/>
+      <c r="B10" s="27">
         <v>112002</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="27"/>
-    </row>
-    <row r="11" spans="1:3" ht="18.75">
-      <c r="A11" s="25">
+      <c r="D10" s="26"/>
+    </row>
+    <row r="11" spans="1:4" ht="18.75">
+      <c r="A11" s="68"/>
+      <c r="B11" s="27">
         <v>112003</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="C11" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="27"/>
-    </row>
-    <row r="12" spans="1:3" ht="18.75">
-      <c r="A12" s="25">
+      <c r="D11" s="26"/>
+    </row>
+    <row r="12" spans="1:4" ht="18.75">
+      <c r="A12" s="68"/>
+      <c r="B12" s="27">
         <v>112004</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="C12" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="27"/>
-    </row>
-    <row r="13" spans="1:3" ht="18.75">
-      <c r="A13" s="25">
+      <c r="D12" s="26"/>
+    </row>
+    <row r="13" spans="1:4" ht="18.75">
+      <c r="A13" s="68"/>
+      <c r="B13" s="27">
         <v>112005</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="C13" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="27"/>
-    </row>
-    <row r="14" spans="1:3" ht="18.75">
-      <c r="A14" s="25">
+      <c r="D13" s="26"/>
+    </row>
+    <row r="14" spans="1:4" ht="18.75">
+      <c r="A14" s="68"/>
+      <c r="B14" s="27">
         <v>112006</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="C14" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="27"/>
-    </row>
-    <row r="15" spans="1:3" ht="18.75">
-      <c r="A15" s="25">
+      <c r="D14" s="26"/>
+    </row>
+    <row r="15" spans="1:4" ht="18.75">
+      <c r="A15" s="68"/>
+      <c r="B15" s="27">
         <v>112007</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="C15" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="27"/>
-    </row>
-    <row r="16" spans="1:3" ht="18.75">
-      <c r="A16" s="25">
+      <c r="D15" s="26"/>
+    </row>
+    <row r="16" spans="1:4" ht="18.75">
+      <c r="A16" s="68"/>
+      <c r="B16" s="27">
         <v>112008</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="C16" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="27"/>
-    </row>
-    <row r="17" spans="1:3" ht="18.75">
-      <c r="A17" s="31">
+      <c r="D16" s="26"/>
+    </row>
+    <row r="17" spans="1:4" ht="18.75">
+      <c r="A17" s="68"/>
+      <c r="B17" s="56">
         <v>112009</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="C17" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="27"/>
-    </row>
-    <row r="18" spans="1:3" ht="18.75">
-      <c r="A18" s="31">
+      <c r="D17" s="26"/>
+    </row>
+    <row r="18" spans="1:4" ht="18.75">
+      <c r="A18" s="68"/>
+      <c r="B18" s="56">
         <v>112010</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="C18" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="27"/>
-    </row>
-    <row r="19" spans="1:3" ht="18.75">
-      <c r="A19" s="31">
+      <c r="D18" s="26"/>
+    </row>
+    <row r="19" spans="1:4" ht="18.75">
+      <c r="A19" s="68"/>
+      <c r="B19" s="56">
         <v>112011</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="C19" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="27"/>
-    </row>
-    <row r="20" spans="1:3" ht="18.75">
-      <c r="A20" s="31">
+      <c r="D19" s="26"/>
+    </row>
+    <row r="20" spans="1:4" ht="18.75">
+      <c r="A20" s="68"/>
+      <c r="B20" s="56">
         <v>112012</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="C20" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="27"/>
-    </row>
-    <row r="21" spans="1:3" ht="18.75">
-      <c r="A21" s="25">
+      <c r="D20" s="26"/>
+    </row>
+    <row r="21" spans="1:4" ht="18.75">
+      <c r="A21" s="68"/>
+      <c r="B21" s="27">
         <v>113</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="C21" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="27"/>
-    </row>
-    <row r="22" spans="1:3" ht="18.75">
-      <c r="A22" s="33">
+      <c r="D21" s="26"/>
+    </row>
+    <row r="22" spans="1:4" ht="18.75">
+      <c r="A22" s="68"/>
+      <c r="B22" s="30">
         <v>114</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="C22" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="27"/>
-    </row>
-    <row r="23" spans="1:3" ht="18.75">
-      <c r="A23" s="33">
+      <c r="D22" s="26"/>
+    </row>
+    <row r="23" spans="1:4" ht="18.75">
+      <c r="A23" s="68"/>
+      <c r="B23" s="30">
         <v>114001</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="C23" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="D23" s="31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="18.75">
-      <c r="A24" s="25">
+    <row r="24" spans="1:4" ht="18.75">
+      <c r="A24" s="68"/>
+      <c r="B24" s="27">
         <v>114002</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="C24" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="27"/>
-    </row>
-    <row r="25" spans="1:3" ht="18.75">
-      <c r="A25" s="36">
+      <c r="D24" s="26"/>
+    </row>
+    <row r="25" spans="1:4" ht="18.75">
+      <c r="A25" s="68"/>
+      <c r="B25" s="33">
         <v>114003</v>
       </c>
-      <c r="B25" s="37" t="s">
+      <c r="C25" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="27"/>
-    </row>
-    <row r="26" spans="1:3" ht="18.75">
-      <c r="A26" s="33">
+      <c r="D25" s="26"/>
+    </row>
+    <row r="26" spans="1:4" ht="18.75">
+      <c r="A26" s="68"/>
+      <c r="B26" s="30">
         <v>115</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="C26" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="27"/>
-    </row>
-    <row r="27" spans="1:3" ht="18.75">
-      <c r="A27" s="25">
+      <c r="D26" s="26"/>
+    </row>
+    <row r="27" spans="1:4" ht="18.75">
+      <c r="A27" s="68"/>
+      <c r="B27" s="27">
         <v>115001</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="C27" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="27"/>
-    </row>
-    <row r="28" spans="1:3" ht="18.75">
-      <c r="A28" s="25">
+      <c r="D27" s="26"/>
+    </row>
+    <row r="28" spans="1:4" ht="18.75">
+      <c r="A28" s="68"/>
+      <c r="B28" s="27">
         <v>116</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="C28" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="27"/>
-    </row>
-    <row r="29" spans="1:3" ht="18.75">
-      <c r="A29" s="36">
+      <c r="D28" s="26"/>
+    </row>
+    <row r="29" spans="1:4" ht="18.75">
+      <c r="A29" s="68"/>
+      <c r="B29" s="33">
         <v>116001</v>
       </c>
-      <c r="B29" s="37" t="s">
+      <c r="C29" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="27"/>
-    </row>
-    <row r="30" spans="1:3" ht="18.75">
-      <c r="A30" s="36">
+      <c r="D29" s="26"/>
+    </row>
+    <row r="30" spans="1:4" ht="18.75">
+      <c r="A30" s="68"/>
+      <c r="B30" s="33">
         <v>116002</v>
       </c>
-      <c r="B30" s="38" t="s">
+      <c r="C30" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="27"/>
-    </row>
-    <row r="31" spans="1:3" ht="18.75">
-      <c r="A31" s="36">
+      <c r="D30" s="26"/>
+    </row>
+    <row r="31" spans="1:4" ht="18.75">
+      <c r="A31" s="68"/>
+      <c r="B31" s="33">
         <v>116003</v>
       </c>
-      <c r="B31" s="37" t="s">
+      <c r="C31" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="27"/>
-    </row>
-    <row r="32" spans="1:3" ht="18.75">
-      <c r="A32" s="25">
+      <c r="D31" s="26"/>
+    </row>
+    <row r="32" spans="1:4" ht="18.75">
+      <c r="A32" s="68"/>
+      <c r="B32" s="27">
         <v>117</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="C32" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="27"/>
-    </row>
-    <row r="33" spans="1:3" ht="18.75">
-      <c r="A33" s="25">
+      <c r="D32" s="26"/>
+    </row>
+    <row r="33" spans="1:4" ht="18.75">
+      <c r="A33" s="68"/>
+      <c r="B33" s="27">
         <v>118</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="C33" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="27"/>
-    </row>
-    <row r="34" spans="1:3" ht="18.75">
-      <c r="A34" s="36">
+      <c r="D33" s="26"/>
+    </row>
+    <row r="34" spans="1:4" ht="18.75">
+      <c r="A34" s="68"/>
+      <c r="B34" s="33">
         <v>118001</v>
       </c>
-      <c r="B34" s="38" t="s">
+      <c r="C34" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="27"/>
-    </row>
-    <row r="35" spans="1:3" ht="18.75">
-      <c r="A35" s="36">
+      <c r="D34" s="26"/>
+    </row>
+    <row r="35" spans="1:4" ht="18.75">
+      <c r="A35" s="68"/>
+      <c r="B35" s="33">
         <v>1180010001</v>
       </c>
-      <c r="B35" s="38" t="s">
+      <c r="C35" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="D35" s="26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="18.75">
-      <c r="A36" s="36">
+    <row r="36" spans="1:4" ht="18.75">
+      <c r="A36" s="68"/>
+      <c r="B36" s="33">
         <v>1180010002</v>
       </c>
-      <c r="B36" s="38" t="s">
+      <c r="C36" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="27" t="s">
+      <c r="D36" s="26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="18.75">
-      <c r="A37" s="33">
+    <row r="37" spans="1:4" ht="18.75">
+      <c r="A37" s="68"/>
+      <c r="B37" s="30">
         <v>119</v>
       </c>
-      <c r="B37" s="39" t="s">
+      <c r="C37" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="27"/>
-    </row>
-    <row r="38" spans="1:3" ht="18.75">
-      <c r="A38" s="25">
+      <c r="D37" s="26"/>
+    </row>
+    <row r="38" spans="1:4" ht="18.75">
+      <c r="A38" s="69" t="s">
+        <v>312</v>
+      </c>
+      <c r="B38" s="27">
         <v>151</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="C38" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="27"/>
-    </row>
-    <row r="39" spans="1:3" ht="18.75">
-      <c r="A39" s="25">
+      <c r="D38" s="26"/>
+    </row>
+    <row r="39" spans="1:4" ht="18.75">
+      <c r="A39" s="69"/>
+      <c r="B39" s="27">
         <v>151001</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="C39" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="27"/>
-    </row>
-    <row r="40" spans="1:3" ht="18.75">
-      <c r="A40" s="25">
+      <c r="D39" s="26"/>
+    </row>
+    <row r="40" spans="1:4" ht="18.75">
+      <c r="A40" s="69"/>
+      <c r="B40" s="27">
         <v>151002</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="C40" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="C40" s="27"/>
-    </row>
-    <row r="41" spans="1:3" ht="18.75">
-      <c r="A41" s="25">
+      <c r="D40" s="26"/>
+    </row>
+    <row r="41" spans="1:4" ht="18.75">
+      <c r="A41" s="69"/>
+      <c r="B41" s="27">
         <v>151003</v>
       </c>
-      <c r="B41" s="26" t="s">
+      <c r="C41" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="C41" s="27"/>
-    </row>
-    <row r="42" spans="1:3" ht="18.75">
-      <c r="A42" s="25">
+      <c r="D41" s="26"/>
+    </row>
+    <row r="42" spans="1:4" ht="18.75">
+      <c r="A42" s="69"/>
+      <c r="B42" s="27">
         <v>151004</v>
       </c>
-      <c r="B42" s="28" t="s">
+      <c r="C42" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="C42" s="27"/>
-    </row>
-    <row r="43" spans="1:3" ht="18.75">
-      <c r="A43" s="25">
+      <c r="D42" s="26"/>
+    </row>
+    <row r="43" spans="1:4" ht="18.75">
+      <c r="A43" s="69"/>
+      <c r="B43" s="27">
         <v>151005</v>
       </c>
-      <c r="B43" s="26" t="s">
+      <c r="C43" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="C43" s="27"/>
-    </row>
-    <row r="44" spans="1:3" ht="18.75">
-      <c r="A44" s="25">
+      <c r="D43" s="26"/>
+    </row>
+    <row r="44" spans="1:4" ht="18.75">
+      <c r="A44" s="69"/>
+      <c r="B44" s="27">
         <v>151006</v>
       </c>
-      <c r="B44" s="26" t="s">
+      <c r="C44" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="27"/>
-    </row>
-    <row r="45" spans="1:3" ht="18.75">
-      <c r="A45" s="25">
+      <c r="D44" s="26"/>
+    </row>
+    <row r="45" spans="1:4" ht="18.75">
+      <c r="A45" s="69"/>
+      <c r="B45" s="27">
         <v>151007</v>
       </c>
-      <c r="B45" s="28" t="s">
+      <c r="C45" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="C45" s="27"/>
-    </row>
-    <row r="46" spans="1:3" ht="18.75">
-      <c r="A46" s="25">
+      <c r="D45" s="26"/>
+    </row>
+    <row r="46" spans="1:4" ht="18.75">
+      <c r="A46" s="69"/>
+      <c r="B46" s="27">
         <v>152</v>
       </c>
-      <c r="B46" s="28" t="s">
+      <c r="C46" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="C46" s="27"/>
-    </row>
-    <row r="47" spans="1:3" ht="18.75">
-      <c r="A47" s="25">
+      <c r="D46" s="26"/>
+    </row>
+    <row r="47" spans="1:4" ht="18.75">
+      <c r="A47" s="69"/>
+      <c r="B47" s="27">
         <v>153</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="C47" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="27"/>
-    </row>
-    <row r="48" spans="1:3" ht="18.75">
-      <c r="A48" s="33">
+      <c r="D47" s="26"/>
+    </row>
+    <row r="48" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A48" s="63" t="s">
+        <v>313</v>
+      </c>
+      <c r="B48" s="30">
         <v>211</v>
       </c>
-      <c r="B48" s="34" t="s">
+      <c r="C48" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="C48" s="27"/>
-    </row>
-    <row r="49" spans="1:3" ht="18.75">
-      <c r="A49" s="25">
+      <c r="D48" s="26"/>
+    </row>
+    <row r="49" spans="1:4" ht="18.75">
+      <c r="A49" s="63"/>
+      <c r="B49" s="27">
         <v>211001</v>
       </c>
-      <c r="B49" s="28" t="s">
+      <c r="C49" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="C49" s="35" t="s">
+      <c r="D49" s="31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="18.75">
-      <c r="A50" s="33">
+    <row r="50" spans="1:4" ht="18.75">
+      <c r="A50" s="63"/>
+      <c r="B50" s="30">
         <v>212</v>
       </c>
-      <c r="B50" s="34" t="s">
+      <c r="C50" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="C50" s="27"/>
-    </row>
-    <row r="51" spans="1:3" ht="18.75">
-      <c r="A51" s="25">
+      <c r="D50" s="26"/>
+    </row>
+    <row r="51" spans="1:4" ht="18.75">
+      <c r="A51" s="63"/>
+      <c r="B51" s="27">
         <v>212001</v>
       </c>
-      <c r="B51" s="28" t="s">
+      <c r="C51" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="C51" s="27"/>
-    </row>
-    <row r="52" spans="1:3" ht="18.75">
-      <c r="A52" s="25">
+      <c r="D51" s="26"/>
+    </row>
+    <row r="52" spans="1:4" ht="18.75">
+      <c r="A52" s="63"/>
+      <c r="B52" s="27">
         <v>213</v>
       </c>
-      <c r="B52" s="28" t="s">
+      <c r="C52" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C52" s="27"/>
-    </row>
-    <row r="53" spans="1:3" ht="18.75">
-      <c r="A53" s="36">
+      <c r="D52" s="26"/>
+    </row>
+    <row r="53" spans="1:4" ht="18.75">
+      <c r="A53" s="63"/>
+      <c r="B53" s="33">
         <v>213001</v>
       </c>
-      <c r="B53" s="37" t="s">
+      <c r="C53" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="27"/>
-    </row>
-    <row r="54" spans="1:3" ht="18.75">
-      <c r="A54" s="36">
+      <c r="D53" s="26"/>
+    </row>
+    <row r="54" spans="1:4" ht="18.75">
+      <c r="A54" s="63"/>
+      <c r="B54" s="33">
         <v>2130010001</v>
       </c>
-      <c r="B54" s="38" t="s">
+      <c r="C54" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="C54" s="27"/>
-    </row>
-    <row r="55" spans="1:3" ht="18.75">
-      <c r="A55" s="36">
+      <c r="D54" s="26"/>
+    </row>
+    <row r="55" spans="1:4" ht="18.75">
+      <c r="A55" s="63"/>
+      <c r="B55" s="33">
         <v>213002</v>
       </c>
-      <c r="B55" s="38" t="s">
+      <c r="C55" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="C55" s="27"/>
-    </row>
-    <row r="56" spans="1:3" ht="18.75">
-      <c r="A56" s="36">
+      <c r="D55" s="26"/>
+    </row>
+    <row r="56" spans="1:4" ht="18.75">
+      <c r="A56" s="63"/>
+      <c r="B56" s="33">
         <v>2130020001</v>
       </c>
-      <c r="B56" s="37" t="s">
+      <c r="C56" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="C56" s="27"/>
-    </row>
-    <row r="57" spans="1:3" ht="18.75">
-      <c r="A57" s="36">
+      <c r="D56" s="26"/>
+    </row>
+    <row r="57" spans="1:4" ht="18.75">
+      <c r="A57" s="63"/>
+      <c r="B57" s="33">
         <v>2130020002</v>
       </c>
-      <c r="B57" s="37" t="s">
+      <c r="C57" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="C57" s="27"/>
-    </row>
-    <row r="58" spans="1:3" ht="18.75">
-      <c r="A58" s="36">
+      <c r="D57" s="26"/>
+    </row>
+    <row r="58" spans="1:4" ht="18.75">
+      <c r="A58" s="63"/>
+      <c r="B58" s="33">
         <v>2130020003</v>
       </c>
-      <c r="B58" s="37" t="s">
+      <c r="C58" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="C58" s="27"/>
-    </row>
-    <row r="59" spans="1:3" ht="18.75">
-      <c r="A59" s="36">
+      <c r="D58" s="26"/>
+    </row>
+    <row r="59" spans="1:4" ht="18.75">
+      <c r="A59" s="63"/>
+      <c r="B59" s="33">
         <v>2130020004</v>
       </c>
-      <c r="B59" s="38" t="s">
+      <c r="C59" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="C59" s="27" t="s">
+      <c r="D59" s="26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="18.75">
-      <c r="A60" s="36">
+    <row r="60" spans="1:4" ht="18.75">
+      <c r="A60" s="63"/>
+      <c r="B60" s="33">
         <v>2130020005</v>
       </c>
-      <c r="B60" s="38" t="s">
+      <c r="C60" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="C60" s="27" t="s">
+      <c r="D60" s="26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="18.75">
-      <c r="A61" s="36">
+    <row r="61" spans="1:4" ht="18.75">
+      <c r="A61" s="63"/>
+      <c r="B61" s="33">
         <v>213003</v>
       </c>
-      <c r="B61" s="37" t="s">
+      <c r="C61" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="C61" s="27"/>
-    </row>
-    <row r="62" spans="1:3" ht="18.75">
-      <c r="A62" s="25">
+      <c r="D61" s="26"/>
+    </row>
+    <row r="62" spans="1:4" ht="18.75">
+      <c r="A62" s="63"/>
+      <c r="B62" s="27">
         <v>214</v>
       </c>
-      <c r="B62" s="26" t="s">
+      <c r="C62" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="C62" s="27"/>
-    </row>
-    <row r="63" spans="1:3" ht="18.75">
-      <c r="A63" s="25">
+      <c r="D62" s="26"/>
+    </row>
+    <row r="63" spans="1:4" ht="18.75">
+      <c r="A63" s="63"/>
+      <c r="B63" s="27">
         <v>215</v>
       </c>
-      <c r="B63" s="26" t="s">
+      <c r="C63" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="C63" s="27"/>
-    </row>
-    <row r="64" spans="1:3" ht="18.75">
-      <c r="A64" s="25">
+      <c r="D63" s="26"/>
+    </row>
+    <row r="64" spans="1:4" ht="18.75">
+      <c r="A64" s="63"/>
+      <c r="B64" s="27">
         <v>216</v>
       </c>
-      <c r="B64" s="28" t="s">
+      <c r="C64" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C64" s="27"/>
-    </row>
-    <row r="65" spans="1:3" ht="18.75">
-      <c r="A65" s="25">
+      <c r="D64" s="26"/>
+    </row>
+    <row r="65" spans="1:4" ht="18.75">
+      <c r="A65" s="63"/>
+      <c r="B65" s="27">
         <v>217</v>
       </c>
-      <c r="B65" s="28" t="s">
+      <c r="C65" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C65" s="27"/>
-    </row>
-    <row r="66" spans="1:3" ht="18.75">
-      <c r="A66" s="40">
+      <c r="D65" s="26"/>
+    </row>
+    <row r="66" spans="1:4" ht="18.75">
+      <c r="A66" s="64" t="s">
+        <v>314</v>
+      </c>
+      <c r="B66" s="35">
         <v>251</v>
       </c>
-      <c r="B66" s="41" t="s">
+      <c r="C66" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="C66" s="27"/>
-    </row>
-    <row r="67" spans="1:3" ht="18.75">
-      <c r="A67" s="40">
+      <c r="D66" s="26"/>
+    </row>
+    <row r="67" spans="1:4" ht="18.75">
+      <c r="A67" s="64"/>
+      <c r="B67" s="35">
         <v>252</v>
       </c>
-      <c r="B67" s="41" t="s">
+      <c r="C67" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="C67" s="27"/>
-    </row>
-    <row r="68" spans="1:3" ht="18.75">
-      <c r="A68" s="40">
+      <c r="D67" s="26"/>
+    </row>
+    <row r="68" spans="1:4" ht="18.75">
+      <c r="A68" s="64"/>
+      <c r="B68" s="35">
         <v>253</v>
       </c>
-      <c r="B68" s="41" t="s">
+      <c r="C68" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="C68" s="27"/>
-    </row>
-    <row r="69" spans="1:3" ht="18.75">
-      <c r="A69" s="25">
+      <c r="D68" s="26"/>
+    </row>
+    <row r="69" spans="1:4" ht="18.75">
+      <c r="A69" s="64"/>
+      <c r="B69" s="27">
         <v>254</v>
       </c>
-      <c r="B69" s="28" t="s">
+      <c r="C69" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="C69" s="27"/>
-    </row>
-    <row r="70" spans="1:3" ht="18.75">
-      <c r="A70" s="25">
+      <c r="D69" s="26"/>
+    </row>
+    <row r="70" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A70" s="65" t="s">
+        <v>315</v>
+      </c>
+      <c r="B70" s="27">
         <v>311</v>
       </c>
-      <c r="B70" s="26" t="s">
+      <c r="C70" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C70" s="27"/>
-    </row>
-    <row r="71" spans="1:3" ht="18.75">
-      <c r="A71" s="25">
+      <c r="D70" s="26"/>
+    </row>
+    <row r="71" spans="1:4" ht="18.75">
+      <c r="A71" s="65"/>
+      <c r="B71" s="27">
         <v>312</v>
       </c>
-      <c r="B71" s="28" t="s">
+      <c r="C71" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C71" s="27"/>
-    </row>
-    <row r="72" spans="1:3" ht="18.75">
-      <c r="A72" s="25">
+      <c r="D71" s="26"/>
+    </row>
+    <row r="72" spans="1:4" ht="18.75">
+      <c r="A72" s="65"/>
+      <c r="B72" s="27">
         <v>313</v>
       </c>
-      <c r="B72" s="28" t="s">
+      <c r="C72" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="C72" s="27"/>
-    </row>
-    <row r="73" spans="1:3" ht="18.75">
-      <c r="A73" s="25">
+      <c r="D72" s="26"/>
+    </row>
+    <row r="73" spans="1:4" ht="18.75">
+      <c r="A73" s="65"/>
+      <c r="B73" s="27">
         <v>314</v>
       </c>
-      <c r="B73" s="28" t="s">
+      <c r="C73" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C73" s="27"/>
-    </row>
-    <row r="74" spans="1:3" ht="18.75">
-      <c r="A74" s="25">
+      <c r="D73" s="26"/>
+    </row>
+    <row r="74" spans="1:4" ht="18.75">
+      <c r="A74" s="65"/>
+      <c r="B74" s="27">
         <v>315</v>
       </c>
-      <c r="B74" s="28" t="s">
+      <c r="C74" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="C74" s="27"/>
-    </row>
-    <row r="75" spans="1:3" ht="18.75">
-      <c r="A75" s="25">
+      <c r="D74" s="26"/>
+    </row>
+    <row r="75" spans="1:4" ht="18.75">
+      <c r="A75" s="59" t="s">
+        <v>295</v>
+      </c>
+      <c r="B75" s="27">
         <v>411</v>
       </c>
-      <c r="B75" s="26" t="s">
+      <c r="C75" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="C75" s="27"/>
-    </row>
-    <row r="76" spans="1:3" ht="18.75">
-      <c r="A76" s="25">
+      <c r="D75" s="26"/>
+    </row>
+    <row r="76" spans="1:4" ht="18.75">
+      <c r="A76" s="59"/>
+      <c r="B76" s="27">
         <v>411001</v>
       </c>
-      <c r="B76" s="26" t="s">
+      <c r="C76" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="C76" s="27"/>
-    </row>
-    <row r="77" spans="1:3" ht="18.75">
-      <c r="A77" s="25">
+      <c r="D76" s="26"/>
+    </row>
+    <row r="77" spans="1:4" ht="18.75">
+      <c r="A77" s="59"/>
+      <c r="B77" s="27">
         <v>412</v>
       </c>
-      <c r="B77" s="28" t="s">
+      <c r="C77" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="C77" s="27"/>
-    </row>
-    <row r="78" spans="1:3" ht="18.75">
-      <c r="A78" s="25">
+      <c r="D77" s="26"/>
+    </row>
+    <row r="78" spans="1:4" ht="18.75">
+      <c r="A78" s="59"/>
+      <c r="B78" s="27">
         <v>412001</v>
       </c>
-      <c r="B78" s="26" t="s">
+      <c r="C78" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="C78" s="27"/>
-    </row>
-    <row r="79" spans="1:3" ht="18.75">
-      <c r="A79" s="25">
+      <c r="D78" s="26"/>
+    </row>
+    <row r="79" spans="1:4" ht="18.75">
+      <c r="A79" s="59"/>
+      <c r="B79" s="27">
         <v>412002</v>
       </c>
-      <c r="B79" s="26" t="s">
+      <c r="C79" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="C79" s="27"/>
-    </row>
-    <row r="80" spans="1:3" ht="18.75">
-      <c r="A80" s="25">
+      <c r="D79" s="26"/>
+    </row>
+    <row r="80" spans="1:4" ht="18.75">
+      <c r="A80" s="59" t="s">
+        <v>316</v>
+      </c>
+      <c r="B80" s="27">
         <v>451</v>
       </c>
-      <c r="B80" s="26" t="s">
+      <c r="C80" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="C80" s="27"/>
-    </row>
-    <row r="81" spans="1:3" ht="18.75">
-      <c r="A81" s="36">
+      <c r="D80" s="26"/>
+    </row>
+    <row r="81" spans="1:4" ht="18.75">
+      <c r="A81" s="59"/>
+      <c r="B81" s="33">
         <v>451001</v>
       </c>
-      <c r="B81" s="38" t="s">
+      <c r="C81" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="C81" s="27"/>
-    </row>
-    <row r="82" spans="1:3" ht="18.75">
-      <c r="A82" s="36">
+      <c r="D81" s="26"/>
+    </row>
+    <row r="82" spans="1:4" ht="18.75">
+      <c r="A82" s="59"/>
+      <c r="B82" s="33">
         <v>451002</v>
       </c>
-      <c r="B82" s="37" t="s">
+      <c r="C82" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="C82" s="27"/>
-    </row>
-    <row r="83" spans="1:3" ht="18.75">
-      <c r="A83" s="25">
+      <c r="D82" s="26"/>
+    </row>
+    <row r="83" spans="1:4" ht="18.75">
+      <c r="A83" s="59"/>
+      <c r="B83" s="27">
         <v>452</v>
       </c>
-      <c r="B83" s="28" t="s">
+      <c r="C83" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="C83" s="27"/>
-    </row>
-    <row r="84" spans="1:3" ht="18.75">
-      <c r="A84" s="25">
+      <c r="D83" s="26"/>
+    </row>
+    <row r="84" spans="1:4" ht="18.75">
+      <c r="A84" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="B84" s="27">
         <v>551</v>
       </c>
-      <c r="B84" s="28" t="s">
+      <c r="C84" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="C84" s="27"/>
-    </row>
-    <row r="85" spans="1:3" ht="131.25">
-      <c r="A85" s="36">
+      <c r="D84" s="26"/>
+    </row>
+    <row r="85" spans="1:4" ht="131.25">
+      <c r="A85" s="60" t="s">
+        <v>322</v>
+      </c>
+      <c r="B85" s="33">
         <v>552</v>
       </c>
-      <c r="B85" s="38" t="s">
+      <c r="C85" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="C85" s="42" t="s">
+      <c r="D85" s="36" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="18.75">
-      <c r="A86" s="36">
+    <row r="86" spans="1:4" ht="18.75">
+      <c r="A86" s="61"/>
+      <c r="B86" s="33">
         <v>552001</v>
       </c>
-      <c r="B86" s="37" t="s">
+      <c r="C86" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="C86" s="27" t="s">
+      <c r="D86" s="26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="18.75">
-      <c r="A87" s="36">
+    <row r="87" spans="1:4" ht="18.75">
+      <c r="A87" s="62"/>
+      <c r="B87" s="33">
         <v>552002</v>
       </c>
-      <c r="B87" s="37" t="s">
+      <c r="C87" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="C87" s="27" t="s">
+      <c r="D87" s="26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="18.75">
-      <c r="A88" s="36">
+    <row r="88" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A88" s="59" t="s">
+        <v>317</v>
+      </c>
+      <c r="B88" s="33">
         <v>610</v>
       </c>
-      <c r="B88" s="38" t="s">
+      <c r="C88" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="C88" s="27"/>
-    </row>
-    <row r="89" spans="1:3" ht="18.75">
-      <c r="A89" s="36">
+      <c r="D88" s="26"/>
+    </row>
+    <row r="89" spans="1:4" ht="18.75">
+      <c r="A89" s="59"/>
+      <c r="B89" s="33">
         <v>610001</v>
       </c>
-      <c r="B89" s="38" t="s">
+      <c r="C89" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="C89" s="27"/>
-    </row>
-    <row r="90" spans="1:3" ht="18.75">
-      <c r="A90" s="36">
+      <c r="D89" s="26"/>
+    </row>
+    <row r="90" spans="1:4" ht="18.75">
+      <c r="A90" s="59"/>
+      <c r="B90" s="33">
         <v>610002</v>
       </c>
-      <c r="B90" s="37" t="s">
+      <c r="C90" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="C90" s="27"/>
-    </row>
-    <row r="91" spans="1:3" ht="18.75">
-      <c r="A91" s="36">
+      <c r="D90" s="26"/>
+    </row>
+    <row r="91" spans="1:4" ht="18.75">
+      <c r="A91" s="59"/>
+      <c r="B91" s="33">
         <v>610003</v>
       </c>
-      <c r="B91" s="37" t="s">
+      <c r="C91" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="C91" s="27"/>
-    </row>
-    <row r="92" spans="1:3" ht="18.75">
-      <c r="A92" s="36">
+      <c r="D91" s="26"/>
+    </row>
+    <row r="92" spans="1:4" ht="18.75">
+      <c r="A92" s="59"/>
+      <c r="B92" s="33">
         <v>610004</v>
       </c>
-      <c r="B92" s="37" t="s">
+      <c r="C92" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="C92" s="27"/>
-    </row>
-    <row r="93" spans="1:3" ht="18.75">
-      <c r="A93" s="36">
+      <c r="D92" s="26"/>
+    </row>
+    <row r="93" spans="1:4" ht="18.75">
+      <c r="A93" s="59"/>
+      <c r="B93" s="33">
         <v>610005</v>
       </c>
-      <c r="B93" s="37" t="s">
+      <c r="C93" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="C93" s="27"/>
-    </row>
-    <row r="94" spans="1:3" ht="18.75">
-      <c r="A94" s="36">
+      <c r="D93" s="26"/>
+    </row>
+    <row r="94" spans="1:4" ht="18.75">
+      <c r="A94" s="59"/>
+      <c r="B94" s="33">
         <v>610006</v>
       </c>
-      <c r="B94" s="38" t="s">
+      <c r="C94" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="C94" s="27"/>
-    </row>
-    <row r="95" spans="1:3" ht="18.75">
-      <c r="A95" s="36">
+      <c r="D94" s="26"/>
+    </row>
+    <row r="95" spans="1:4" ht="18.75">
+      <c r="A95" s="59"/>
+      <c r="B95" s="33">
         <v>610007</v>
       </c>
-      <c r="B95" s="38" t="s">
+      <c r="C95" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="C95" s="27"/>
-    </row>
-    <row r="96" spans="1:3" ht="18.75">
-      <c r="A96" s="33">
+      <c r="D95" s="26"/>
+    </row>
+    <row r="96" spans="1:4" ht="18.75">
+      <c r="A96" s="59"/>
+      <c r="B96" s="30">
         <v>611</v>
       </c>
-      <c r="B96" s="34" t="s">
+      <c r="C96" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="C96" s="27"/>
-    </row>
-    <row r="97" spans="1:3" ht="18.75">
-      <c r="A97" s="36">
+      <c r="D96" s="26"/>
+    </row>
+    <row r="97" spans="1:4" ht="18.75">
+      <c r="A97" s="59"/>
+      <c r="B97" s="33">
         <v>611001</v>
       </c>
-      <c r="B97" s="37" t="s">
+      <c r="C97" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="C97" s="27"/>
-    </row>
-    <row r="98" spans="1:3" ht="18.75">
-      <c r="A98" s="36">
+      <c r="D97" s="26"/>
+    </row>
+    <row r="98" spans="1:4" ht="18.75">
+      <c r="A98" s="59"/>
+      <c r="B98" s="33">
         <v>611002</v>
       </c>
-      <c r="B98" s="37" t="s">
+      <c r="C98" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="C98" s="27"/>
-    </row>
-    <row r="99" spans="1:3" ht="18.75">
-      <c r="A99" s="36">
+      <c r="D98" s="26"/>
+    </row>
+    <row r="99" spans="1:4" ht="18.75">
+      <c r="A99" s="59"/>
+      <c r="B99" s="33">
         <v>611003</v>
       </c>
-      <c r="B99" s="38" t="s">
+      <c r="C99" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="C99" s="27"/>
-    </row>
-    <row r="100" spans="1:3" ht="18.75">
-      <c r="A100" s="36">
+      <c r="D99" s="26"/>
+    </row>
+    <row r="100" spans="1:4" ht="18.75">
+      <c r="A100" s="59"/>
+      <c r="B100" s="33">
         <v>611004</v>
       </c>
-      <c r="B100" s="37" t="s">
+      <c r="C100" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="C100" s="27"/>
-    </row>
-    <row r="101" spans="1:3" ht="18.75">
-      <c r="A101" s="36">
+      <c r="D100" s="26"/>
+    </row>
+    <row r="101" spans="1:4" ht="18.75">
+      <c r="A101" s="59"/>
+      <c r="B101" s="33">
         <v>611005</v>
       </c>
-      <c r="B101" s="37" t="s">
+      <c r="C101" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="C101" s="27"/>
-    </row>
-    <row r="102" spans="1:3" ht="18.75">
-      <c r="A102" s="36">
+      <c r="D101" s="26"/>
+    </row>
+    <row r="102" spans="1:4" ht="18.75">
+      <c r="A102" s="59"/>
+      <c r="B102" s="33">
         <v>611006</v>
       </c>
-      <c r="B102" s="38" t="s">
+      <c r="C102" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="C102" s="27"/>
-    </row>
-    <row r="103" spans="1:3" ht="18.75">
-      <c r="A103" s="36">
+      <c r="D102" s="26"/>
+    </row>
+    <row r="103" spans="1:4" ht="18.75">
+      <c r="A103" s="59"/>
+      <c r="B103" s="33">
         <v>611007</v>
       </c>
-      <c r="B103" s="37" t="s">
+      <c r="C103" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="C103" s="27"/>
-    </row>
-    <row r="104" spans="1:3" ht="18.75">
-      <c r="A104" s="36">
+      <c r="D103" s="26"/>
+    </row>
+    <row r="104" spans="1:4" ht="18.75">
+      <c r="A104" s="59"/>
+      <c r="B104" s="33">
         <v>611008</v>
       </c>
-      <c r="B104" s="37" t="s">
+      <c r="C104" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="C104" s="27"/>
-    </row>
-    <row r="105" spans="1:3" ht="18.75">
-      <c r="A105" s="36">
+      <c r="D104" s="26"/>
+    </row>
+    <row r="105" spans="1:4" ht="18.75">
+      <c r="A105" s="59"/>
+      <c r="B105" s="33">
         <v>611009</v>
       </c>
-      <c r="B105" s="37" t="s">
+      <c r="C105" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="C105" s="27"/>
-    </row>
-    <row r="106" spans="1:3" ht="18.75">
-      <c r="A106" s="36">
+      <c r="D105" s="26"/>
+    </row>
+    <row r="106" spans="1:4" ht="18.75">
+      <c r="A106" s="59"/>
+      <c r="B106" s="33">
         <v>611010</v>
       </c>
-      <c r="B106" s="37" t="s">
+      <c r="C106" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="C106" s="27"/>
-    </row>
-    <row r="107" spans="1:3" ht="18.75">
-      <c r="A107" s="36">
+      <c r="D106" s="26"/>
+    </row>
+    <row r="107" spans="1:4" ht="18.75">
+      <c r="A107" s="59"/>
+      <c r="B107" s="33">
         <v>611011</v>
       </c>
-      <c r="B107" s="37" t="s">
+      <c r="C107" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="C107" s="27"/>
-    </row>
-    <row r="108" spans="1:3" ht="18.75">
-      <c r="A108" s="33">
+      <c r="D107" s="26"/>
+    </row>
+    <row r="108" spans="1:4" ht="18.75">
+      <c r="A108" s="59"/>
+      <c r="B108" s="30">
         <v>612</v>
       </c>
-      <c r="B108" s="34" t="s">
+      <c r="C108" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="C108" s="27"/>
-    </row>
-    <row r="109" spans="1:3" ht="18.75">
-      <c r="A109" s="36">
+      <c r="D108" s="26"/>
+    </row>
+    <row r="109" spans="1:4" ht="18.75">
+      <c r="A109" s="59"/>
+      <c r="B109" s="33">
         <v>612001</v>
       </c>
-      <c r="B109" s="38" t="s">
+      <c r="C109" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="C109" s="27"/>
-    </row>
-    <row r="110" spans="1:3" ht="18.75">
-      <c r="A110" s="36">
+      <c r="D109" s="26"/>
+    </row>
+    <row r="110" spans="1:4" ht="18.75">
+      <c r="A110" s="59"/>
+      <c r="B110" s="33">
         <v>612002</v>
       </c>
-      <c r="B110" s="38" t="s">
+      <c r="C110" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="C110" s="27"/>
-    </row>
-    <row r="111" spans="1:3" ht="18.75">
-      <c r="A111" s="36">
+      <c r="D110" s="26"/>
+    </row>
+    <row r="111" spans="1:4" ht="18.75">
+      <c r="A111" s="59"/>
+      <c r="B111" s="33">
         <v>613</v>
       </c>
-      <c r="B111" s="38" t="s">
+      <c r="C111" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="C111" s="27"/>
-    </row>
-    <row r="112" spans="1:3" ht="18.75">
-      <c r="A112" s="36">
+      <c r="D111" s="26"/>
+    </row>
+    <row r="112" spans="1:4" ht="18.75">
+      <c r="A112" s="59"/>
+      <c r="B112" s="33">
         <v>613001</v>
       </c>
-      <c r="B112" s="37" t="s">
+      <c r="C112" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="C112" s="27"/>
-    </row>
-    <row r="113" spans="1:3" ht="18.75">
-      <c r="A113" s="36">
+      <c r="D112" s="26"/>
+    </row>
+    <row r="113" spans="1:4" ht="18.75">
+      <c r="A113" s="59"/>
+      <c r="B113" s="33">
         <v>613002</v>
       </c>
-      <c r="B113" s="37" t="s">
+      <c r="C113" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="C113" s="27"/>
-    </row>
-    <row r="114" spans="1:3" ht="18.75">
-      <c r="A114" s="36">
+      <c r="D113" s="26"/>
+    </row>
+    <row r="114" spans="1:4" ht="18.75">
+      <c r="A114" s="59"/>
+      <c r="B114" s="33">
         <v>613003</v>
       </c>
-      <c r="B114" s="37" t="s">
+      <c r="C114" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="C114" s="27"/>
-    </row>
-    <row r="115" spans="1:3" ht="18.75">
-      <c r="A115" s="36">
+      <c r="D114" s="26"/>
+    </row>
+    <row r="115" spans="1:4" ht="18.75">
+      <c r="A115" s="59" t="s">
+        <v>318</v>
+      </c>
+      <c r="B115" s="33">
         <v>614</v>
       </c>
-      <c r="B115" s="38" t="s">
+      <c r="C115" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="C115" s="27"/>
-    </row>
-    <row r="116" spans="1:3" ht="18.75">
-      <c r="A116" s="36">
+      <c r="D115" s="26"/>
+    </row>
+    <row r="116" spans="1:4" ht="18.75">
+      <c r="A116" s="59"/>
+      <c r="B116" s="33">
         <v>614001</v>
       </c>
-      <c r="B116" s="38" t="s">
+      <c r="C116" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="C116" s="27"/>
-    </row>
-    <row r="117" spans="1:3" ht="18.75">
-      <c r="A117" s="36">
+      <c r="D116" s="26"/>
+    </row>
+    <row r="117" spans="1:4" ht="18.75">
+      <c r="A117" s="59"/>
+      <c r="B117" s="33">
         <v>614002</v>
       </c>
-      <c r="B117" s="38" t="s">
+      <c r="C117" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="C117" s="27"/>
-    </row>
-    <row r="118" spans="1:3" ht="18.75">
-      <c r="A118" s="36">
+      <c r="D117" s="26"/>
+    </row>
+    <row r="118" spans="1:4" ht="18.75">
+      <c r="A118" s="59"/>
+      <c r="B118" s="33">
         <v>614003</v>
       </c>
-      <c r="B118" s="38" t="s">
+      <c r="C118" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="C118" s="27"/>
-    </row>
-    <row r="119" spans="1:3" ht="18.75">
-      <c r="A119" s="25">
+      <c r="D118" s="26"/>
+    </row>
+    <row r="119" spans="1:4" ht="18.75">
+      <c r="A119" s="59" t="s">
+        <v>319</v>
+      </c>
+      <c r="B119" s="27">
         <v>711</v>
       </c>
-      <c r="B119" s="26" t="s">
+      <c r="C119" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="C119" s="27"/>
-    </row>
-    <row r="120" spans="1:3" ht="18.75">
-      <c r="A120" s="25">
+      <c r="D119" s="26"/>
+    </row>
+    <row r="120" spans="1:4" ht="18.75">
+      <c r="A120" s="59"/>
+      <c r="B120" s="27">
         <v>712</v>
       </c>
-      <c r="B120" s="26" t="s">
+      <c r="C120" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="C120" s="27"/>
-    </row>
-    <row r="121" spans="1:3" ht="18.75">
-      <c r="A121" s="25">
+      <c r="D120" s="26"/>
+    </row>
+    <row r="121" spans="1:4" ht="18.75">
+      <c r="A121" s="59"/>
+      <c r="B121" s="27">
         <v>713</v>
       </c>
-      <c r="B121" s="26" t="s">
+      <c r="C121" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="C121" s="27"/>
-    </row>
-    <row r="122" spans="1:3" ht="18.75">
-      <c r="A122" s="25">
+      <c r="D121" s="26"/>
+    </row>
+    <row r="122" spans="1:4" ht="18.75">
+      <c r="A122" s="59"/>
+      <c r="B122" s="27">
         <v>714</v>
       </c>
-      <c r="B122" s="26" t="s">
+      <c r="C122" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C122" s="27"/>
-    </row>
-    <row r="123" spans="1:3" ht="37.5">
-      <c r="A123" s="25">
+      <c r="D122" s="26"/>
+    </row>
+    <row r="123" spans="1:4" ht="37.5">
+      <c r="A123" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="B123" s="27">
         <v>811</v>
       </c>
-      <c r="B123" s="28" t="s">
+      <c r="C123" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="C123" s="35" t="s">
+      <c r="D123" s="31" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="38.25" thickBot="1">
-      <c r="A124" s="43">
+    <row r="124" spans="1:4" ht="38.25" thickBot="1">
+      <c r="A124" s="59"/>
+      <c r="B124" s="37">
         <v>812</v>
       </c>
-      <c r="B124" s="44" t="s">
+      <c r="C124" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="C124" s="45" t="s">
+      <c r="D124" s="38" t="s">
         <v>147</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+  <mergeCells count="13">
+    <mergeCell ref="A48:A65"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A37"/>
+    <mergeCell ref="A38:A47"/>
+    <mergeCell ref="A115:A118"/>
+    <mergeCell ref="A119:A122"/>
+    <mergeCell ref="A123:A124"/>
+    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="A75:A79"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="A88:A114"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4567,13 +4894,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="70" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
@@ -4911,7 +5238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView rightToLeft="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -4943,59 +5270,59 @@
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" ht="132" customHeight="1">
-      <c r="A2" s="54" t="s">
-        <v>309</v>
-      </c>
-      <c r="B2" s="54"/>
+      <c r="A2" s="47" t="s">
+        <v>307</v>
+      </c>
+      <c r="B2" s="47"/>
       <c r="C2" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D2" s="58" t="s">
-        <v>310</v>
+        <v>300</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>308</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
       <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" ht="132.75" customHeight="1">
-      <c r="A3" s="54"/>
-      <c r="B3" s="54" t="s">
-        <v>307</v>
+      <c r="A3" s="47"/>
+      <c r="B3" s="47" t="s">
+        <v>305</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="D3" s="58" t="s">
-        <v>311</v>
+        <v>301</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>309</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:7" ht="180" customHeight="1">
-      <c r="A4" s="54"/>
-      <c r="B4" s="54" t="s">
-        <v>307</v>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47" t="s">
+        <v>305</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="D4" s="58" t="s">
-        <v>312</v>
+        <v>302</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>310</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="54"/>
-      <c r="B5" s="54" t="s">
-        <v>307</v>
+      <c r="A5" s="47"/>
+      <c r="B5" s="47" t="s">
+        <v>305</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="D5" s="58"/>
+        <v>304</v>
+      </c>
+      <c r="D5" s="51"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="12"/>
@@ -5005,13 +5332,13 @@
         <v>223</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:7" ht="112.5">
       <c r="B7" s="10" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>285</v>
@@ -5213,8 +5540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView rightToLeft="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -5247,7 +5574,7 @@
       <c r="B2" s="14" t="s">
         <v>264</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="42" t="s">
         <v>279</v>
       </c>
     </row>
@@ -5255,19 +5582,19 @@
       <c r="B3" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="42" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="50"/>
-      <c r="B4" s="50" t="s">
+      <c r="A4" s="43"/>
+      <c r="B4" s="43" t="s">
         <v>267</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="42" t="s">
         <v>278</v>
       </c>
-      <c r="D4" s="51"/>
+      <c r="D4" s="44"/>
     </row>
     <row r="5" spans="1:7" ht="112.5">
       <c r="B5" s="10" t="s">
@@ -5281,7 +5608,7 @@
       <c r="B6" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="45" t="s">
         <v>269</v>
       </c>
     </row>
@@ -5305,28 +5632,28 @@
       <c r="B9" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="49" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="115.5">
-      <c r="A10" s="53"/>
-      <c r="B10" s="54" t="s">
+      <c r="A10" s="46"/>
+      <c r="B10" s="47" t="s">
         <v>274</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="48" t="s">
         <v>275</v>
       </c>
-      <c r="D10" s="49"/>
+      <c r="D10" s="42"/>
     </row>
     <row r="11" spans="1:7" ht="206.25">
       <c r="B11" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="41" t="s">
         <v>283</v>
       </c>
-      <c r="D11" s="51"/>
+      <c r="D11" s="44"/>
     </row>
     <row r="12" spans="1:7" ht="75">
       <c r="B12" s="10" t="s">
@@ -5368,58 +5695,58 @@
       <c r="C21" s="11"/>
     </row>
     <row r="22" spans="3:3">
-      <c r="C22" s="49"/>
+      <c r="C22" s="42"/>
     </row>
     <row r="23" spans="3:3">
-      <c r="C23" s="49"/>
+      <c r="C23" s="42"/>
     </row>
     <row r="24" spans="3:3">
-      <c r="C24" s="49"/>
+      <c r="C24" s="42"/>
     </row>
     <row r="25" spans="3:3">
-      <c r="C25" s="49"/>
+      <c r="C25" s="42"/>
     </row>
     <row r="26" spans="3:3">
-      <c r="C26" s="49"/>
+      <c r="C26" s="42"/>
     </row>
     <row r="27" spans="3:3">
-      <c r="C27" s="49"/>
+      <c r="C27" s="42"/>
     </row>
     <row r="28" spans="3:3">
-      <c r="C28" s="49"/>
+      <c r="C28" s="42"/>
     </row>
     <row r="29" spans="3:3">
-      <c r="C29" s="49"/>
+      <c r="C29" s="42"/>
     </row>
     <row r="30" spans="3:3">
-      <c r="C30" s="49"/>
+      <c r="C30" s="42"/>
     </row>
     <row r="31" spans="3:3">
-      <c r="C31" s="49"/>
+      <c r="C31" s="42"/>
     </row>
     <row r="32" spans="3:3">
-      <c r="C32" s="49"/>
+      <c r="C32" s="42"/>
     </row>
     <row r="33" spans="3:3">
-      <c r="C33" s="49"/>
+      <c r="C33" s="42"/>
     </row>
     <row r="34" spans="3:3">
-      <c r="C34" s="49"/>
+      <c r="C34" s="42"/>
     </row>
     <row r="35" spans="3:3">
-      <c r="C35" s="49"/>
+      <c r="C35" s="42"/>
     </row>
     <row r="36" spans="3:3">
-      <c r="C36" s="49"/>
+      <c r="C36" s="42"/>
     </row>
     <row r="37" spans="3:3">
-      <c r="C37" s="49"/>
+      <c r="C37" s="42"/>
     </row>
     <row r="38" spans="3:3">
-      <c r="C38" s="49"/>
+      <c r="C38" s="42"/>
     </row>
     <row r="39" spans="3:3">
-      <c r="C39" s="49"/>
+      <c r="C39" s="42"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -5440,7 +5767,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -5448,7 +5775,7 @@
     <col min="1" max="1" width="11" style="14" customWidth="1"/>
     <col min="2" max="2" width="33.7109375" style="14" customWidth="1"/>
     <col min="3" max="3" width="75.7109375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="90.7109375" style="59" customWidth="1"/>
+    <col min="4" max="4" width="90.7109375" style="52" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
@@ -5462,8 +5789,8 @@
       <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="60" t="s">
-        <v>295</v>
+      <c r="D1" s="53" t="s">
+        <v>294</v>
       </c>
       <c r="E1" s="10"/>
       <c r="F1" s="12"/>
@@ -5472,53 +5799,53 @@
       <c r="B2" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="C2" s="57" t="s">
-        <v>290</v>
-      </c>
-      <c r="D2" s="66"/>
+      <c r="C2" s="50" t="s">
+        <v>321</v>
+      </c>
+      <c r="D2" s="71"/>
     </row>
     <row r="3" spans="1:6" ht="65.25" customHeight="1">
       <c r="B3" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="C3" s="50" t="s">
         <v>291</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="D3" s="71"/>
+    </row>
+    <row r="4" spans="1:6" ht="45.75" customHeight="1">
+      <c r="A4" s="43"/>
+      <c r="B4" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="D3" s="66"/>
-    </row>
-    <row r="4" spans="1:6" ht="45.75" customHeight="1">
-      <c r="A4" s="50"/>
-      <c r="B4" s="50" t="s">
+      <c r="C4" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>294</v>
-      </c>
-      <c r="D4" s="66"/>
+      <c r="D4" s="71"/>
     </row>
     <row r="5" spans="1:6" ht="292.5" customHeight="1">
       <c r="B5" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>297</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="204.75" customHeight="1">
       <c r="B6" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="C6" s="52" t="s">
-        <v>299</v>
-      </c>
-      <c r="D6" s="61"/>
+        <v>296</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>297</v>
+      </c>
+      <c r="D6" s="54"/>
     </row>
     <row r="7" spans="1:6" ht="243" customHeight="1">
       <c r="B7" s="10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -5527,16 +5854,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="B9" s="10"/>
-      <c r="C9" s="56"/>
+      <c r="C9" s="49"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="53"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="55"/>
+      <c r="A10" s="46"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="48"/>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" s="10"/>
-      <c r="C11" s="48"/>
+      <c r="C11" s="41"/>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" s="10"/>
@@ -5571,58 +5898,58 @@
       <c r="C21" s="11"/>
     </row>
     <row r="22" spans="3:3">
-      <c r="C22" s="57"/>
+      <c r="C22" s="50"/>
     </row>
     <row r="23" spans="3:3">
-      <c r="C23" s="57"/>
+      <c r="C23" s="50"/>
     </row>
     <row r="24" spans="3:3">
-      <c r="C24" s="57"/>
+      <c r="C24" s="50"/>
     </row>
     <row r="25" spans="3:3">
-      <c r="C25" s="57"/>
+      <c r="C25" s="50"/>
     </row>
     <row r="26" spans="3:3">
-      <c r="C26" s="57"/>
+      <c r="C26" s="50"/>
     </row>
     <row r="27" spans="3:3">
-      <c r="C27" s="57"/>
+      <c r="C27" s="50"/>
     </row>
     <row r="28" spans="3:3">
-      <c r="C28" s="57"/>
+      <c r="C28" s="50"/>
     </row>
     <row r="29" spans="3:3">
-      <c r="C29" s="57"/>
+      <c r="C29" s="50"/>
     </row>
     <row r="30" spans="3:3">
-      <c r="C30" s="57"/>
+      <c r="C30" s="50"/>
     </row>
     <row r="31" spans="3:3">
-      <c r="C31" s="57"/>
+      <c r="C31" s="50"/>
     </row>
     <row r="32" spans="3:3">
-      <c r="C32" s="57"/>
+      <c r="C32" s="50"/>
     </row>
     <row r="33" spans="3:3">
-      <c r="C33" s="57"/>
+      <c r="C33" s="50"/>
     </row>
     <row r="34" spans="3:3">
-      <c r="C34" s="57"/>
+      <c r="C34" s="50"/>
     </row>
     <row r="35" spans="3:3">
-      <c r="C35" s="57"/>
+      <c r="C35" s="50"/>
     </row>
     <row r="36" spans="3:3">
-      <c r="C36" s="57"/>
+      <c r="C36" s="50"/>
     </row>
     <row r="37" spans="3:3">
-      <c r="C37" s="57"/>
+      <c r="C37" s="50"/>
     </row>
     <row r="38" spans="3:3">
-      <c r="C38" s="57"/>
+      <c r="C38" s="50"/>
     </row>
     <row r="39" spans="3:3">
-      <c r="C39" s="57"/>
+      <c r="C39" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>